<commit_message>
Revision with - correction for the calculation of the L matrix (indexing) - set up of PP and Fisheries as 'emptying' source and 'filling' sink of biomass - outputing of data and parameters on screen - not yet functional :(
</commit_message>
<xml_diff>
--- a/CaN.Input.Data.xlsx
+++ b/CaN.Input.Data.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjamin/Documents/Work/CaN/CaN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CB006A-0BF6-1641-84FE-3E68757F8F71}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C5250B6E-4FCB-904B-97A0-72E421B6E439}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6700" yWindow="2980" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{273F929D-1BE0-B64B-9C73-B17798356DE2}"/>
+    <workbookView xWindow="6700" yWindow="2980" windowWidth="28040" windowHeight="17440" activeTab="6" xr2:uid="{273F929D-1BE0-B64B-9C73-B17798356DE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Biomasses" sheetId="1" r:id="rId1"/>
     <sheet name="Landings" sheetId="2" r:id="rId2"/>
     <sheet name="Input.parameters" sheetId="3" r:id="rId3"/>
     <sheet name="Trophic.flows" sheetId="4" r:id="rId4"/>
+    <sheet name="Biomasses.mini" sheetId="5" r:id="rId5"/>
+    <sheet name="Landings.mini" sheetId="6" r:id="rId6"/>
+    <sheet name="Input.parameters.mini" sheetId="7" r:id="rId7"/>
+    <sheet name="Trophic.flows.mini" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="34">
   <si>
     <t>Year</t>
   </si>
@@ -504,7 +508,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB5008E-EAEA-734B-A1C9-2CD9D713586D}">
   <dimension ref="A1:Y27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -615,16 +621,16 @@
         <f>2.5*E2</f>
         <v>41520</v>
       </c>
-      <c r="H2" s="1">
-        <v>3664</v>
+      <c r="H2">
+        <v>16864</v>
       </c>
       <c r="I2" s="1">
         <f>0.6*H2</f>
-        <v>2198.4</v>
+        <v>10118.4</v>
       </c>
       <c r="J2" s="1">
         <f>1.6*H2</f>
-        <v>5862.4000000000005</v>
+        <v>26982.400000000001</v>
       </c>
       <c r="K2" s="1">
         <v>105000</v>
@@ -708,16 +714,16 @@
         <f t="shared" ref="G3:G27" si="3">2.5*E3</f>
         <v>69680</v>
       </c>
-      <c r="H3" s="1">
-        <v>8448</v>
+      <c r="H3">
+        <v>13616</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I27" si="4">0.6*H3</f>
-        <v>5068.8</v>
+        <v>8169.5999999999995</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J27" si="5">1.6*H3</f>
-        <v>13516.800000000001</v>
+        <v>21785.600000000002</v>
       </c>
       <c r="K3" s="1">
         <v>105000</v>
@@ -801,16 +807,16 @@
         <f t="shared" si="3"/>
         <v>58760</v>
       </c>
-      <c r="H4" s="1">
-        <v>6272</v>
+      <c r="H4">
+        <v>7695.99999999999</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="4"/>
-        <v>3763.2</v>
+        <v>4617.599999999994</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="5"/>
-        <v>10035.200000000001</v>
+        <v>12313.599999999984</v>
       </c>
       <c r="K4" s="1">
         <v>105000</v>
@@ -894,16 +900,16 @@
         <f t="shared" si="3"/>
         <v>54440</v>
       </c>
-      <c r="H5" s="1">
-        <v>5392</v>
+      <c r="H5">
+        <v>14640</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="4"/>
-        <v>3235.2</v>
+        <v>8784</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="5"/>
-        <v>8627.2000000000007</v>
+        <v>23424</v>
       </c>
       <c r="K5" s="1">
         <v>105000</v>
@@ -987,16 +993,16 @@
         <f t="shared" si="3"/>
         <v>67040</v>
       </c>
-      <c r="H6" s="1">
-        <v>6016</v>
+      <c r="H6">
+        <v>7008</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="4"/>
-        <v>3609.6</v>
+        <v>4204.8</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="5"/>
-        <v>9625.6</v>
+        <v>11212.800000000001</v>
       </c>
       <c r="K6" s="1">
         <v>105000</v>
@@ -1080,16 +1086,16 @@
         <f t="shared" si="3"/>
         <v>93600</v>
       </c>
-      <c r="H7" s="1">
-        <v>10624</v>
+      <c r="H7">
+        <v>13008</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="4"/>
-        <v>6374.4</v>
+        <v>7804.7999999999993</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="5"/>
-        <v>16998.400000000001</v>
+        <v>20812.800000000003</v>
       </c>
       <c r="K7" s="1">
         <v>105000</v>
@@ -1173,16 +1179,16 @@
         <f t="shared" si="3"/>
         <v>178520</v>
       </c>
-      <c r="H8" s="1">
-        <v>10624</v>
+      <c r="H8">
+        <v>17552</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="4"/>
-        <v>6374.4</v>
+        <v>10531.199999999999</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="5"/>
-        <v>16998.400000000001</v>
+        <v>28083.200000000001</v>
       </c>
       <c r="K8" s="1">
         <v>105000</v>
@@ -1266,16 +1272,16 @@
         <f t="shared" si="3"/>
         <v>143240</v>
       </c>
-      <c r="H9" s="1">
-        <v>8624</v>
+      <c r="H9">
+        <v>16784</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="4"/>
-        <v>5174.3999999999996</v>
+        <v>10070.4</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="5"/>
-        <v>13798.400000000001</v>
+        <v>26854.400000000001</v>
       </c>
       <c r="K9" s="1">
         <v>105000</v>
@@ -1359,16 +1365,16 @@
         <f t="shared" si="3"/>
         <v>96880</v>
       </c>
-      <c r="H10" s="1">
-        <v>9312</v>
+      <c r="H10">
+        <v>19536</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="4"/>
-        <v>5587.2</v>
+        <v>11721.6</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="5"/>
-        <v>14899.2</v>
+        <v>31257.600000000002</v>
       </c>
       <c r="K10" s="1">
         <v>105000</v>
@@ -1452,16 +1458,16 @@
         <f t="shared" si="3"/>
         <v>112560</v>
       </c>
-      <c r="H11" s="1">
-        <v>12800</v>
+      <c r="H11">
+        <v>16191.9999999999</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="4"/>
-        <v>7680</v>
+        <v>9715.1999999999389</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="5"/>
-        <v>20480</v>
+        <v>25907.199999999841</v>
       </c>
       <c r="K11" s="1">
         <v>105000</v>
@@ -1545,16 +1551,16 @@
         <f t="shared" si="3"/>
         <v>101240</v>
       </c>
-      <c r="H12" s="1">
-        <v>11488</v>
+      <c r="H12">
+        <v>17744</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="4"/>
-        <v>6892.8</v>
+        <v>10646.4</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="5"/>
-        <v>18380.8</v>
+        <v>28390.400000000001</v>
       </c>
       <c r="K12" s="1">
         <v>105000</v>
@@ -1638,16 +1644,16 @@
         <f t="shared" si="3"/>
         <v>87520</v>
       </c>
-      <c r="H13" s="1">
-        <v>8272</v>
+      <c r="H13">
+        <v>13104</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="4"/>
-        <v>4963.2</v>
+        <v>7862.4</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="5"/>
-        <v>13235.2</v>
+        <v>20966.400000000001</v>
       </c>
       <c r="K13" s="1">
         <v>105000</v>
@@ -1731,16 +1737,16 @@
         <f t="shared" si="3"/>
         <v>104040</v>
       </c>
-      <c r="H14" s="1">
-        <v>8624</v>
+      <c r="H14">
+        <v>12736</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="4"/>
-        <v>5174.3999999999996</v>
+        <v>7641.5999999999995</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="5"/>
-        <v>13798.400000000001</v>
+        <v>20377.600000000002</v>
       </c>
       <c r="K14" s="1">
         <v>105000</v>
@@ -1824,16 +1830,16 @@
         <f t="shared" si="3"/>
         <v>77920</v>
       </c>
-      <c r="H15" s="1">
-        <v>6272</v>
+      <c r="H15">
+        <v>13104</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="4"/>
-        <v>3763.2</v>
+        <v>7862.4</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="5"/>
-        <v>10035.200000000001</v>
+        <v>20966.400000000001</v>
       </c>
       <c r="K15" s="1">
         <v>105000</v>
@@ -1917,16 +1923,16 @@
         <f t="shared" si="3"/>
         <v>87720</v>
       </c>
-      <c r="H16" s="1">
-        <v>8880</v>
+      <c r="H16">
+        <v>12224</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="4"/>
-        <v>5328</v>
+        <v>7334.4</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="5"/>
-        <v>14208</v>
+        <v>19558.400000000001</v>
       </c>
       <c r="K16" s="1">
         <v>105000</v>
@@ -2010,16 +2016,16 @@
         <f t="shared" si="3"/>
         <v>79440</v>
       </c>
-      <c r="H17" s="1">
-        <v>9760</v>
+      <c r="H17">
+        <v>17184</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="4"/>
-        <v>5856</v>
+        <v>10310.4</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="5"/>
-        <v>15616</v>
+        <v>27494.400000000001</v>
       </c>
       <c r="K17" s="1">
         <v>105000</v>
@@ -2103,16 +2109,16 @@
         <f t="shared" si="3"/>
         <v>91200</v>
       </c>
-      <c r="H18" s="1">
-        <v>13056</v>
+      <c r="H18">
+        <v>25344</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" si="4"/>
-        <v>7833.5999999999995</v>
+        <v>15206.4</v>
       </c>
       <c r="J18" s="1">
         <f t="shared" si="5"/>
-        <v>20889.600000000002</v>
+        <v>40550.400000000001</v>
       </c>
       <c r="K18" s="1">
         <v>105000</v>
@@ -2196,16 +2202,16 @@
         <f t="shared" si="3"/>
         <v>104040</v>
       </c>
-      <c r="H19" s="1">
-        <v>6959.99999999999</v>
+      <c r="H19">
+        <v>17392</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" si="4"/>
-        <v>4175.9999999999936</v>
+        <v>10435.199999999999</v>
       </c>
       <c r="J19" s="1">
         <f t="shared" si="5"/>
-        <v>11135.999999999985</v>
+        <v>27827.200000000001</v>
       </c>
       <c r="K19" s="1">
         <v>105000</v>
@@ -2289,16 +2295,16 @@
         <f t="shared" si="3"/>
         <v>114520</v>
       </c>
-      <c r="H20" s="1">
-        <v>9408</v>
+      <c r="H20">
+        <v>21152</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" si="4"/>
-        <v>5644.8</v>
+        <v>12691.199999999999</v>
       </c>
       <c r="J20" s="1">
         <f t="shared" si="5"/>
-        <v>15052.800000000001</v>
+        <v>33843.200000000004</v>
       </c>
       <c r="K20" s="1">
         <v>105000</v>
@@ -2382,16 +2388,16 @@
         <f t="shared" si="3"/>
         <v>97960</v>
       </c>
-      <c r="H21" s="1">
-        <v>6272</v>
+      <c r="H21">
+        <v>27392</v>
       </c>
       <c r="I21" s="1">
         <f t="shared" si="4"/>
-        <v>3763.2</v>
+        <v>16435.2</v>
       </c>
       <c r="J21" s="1">
         <f t="shared" si="5"/>
-        <v>10035.200000000001</v>
+        <v>43827.200000000004</v>
       </c>
       <c r="K21" s="1">
         <v>105000</v>
@@ -2475,16 +2481,16 @@
         <f t="shared" si="3"/>
         <v>88400</v>
       </c>
-      <c r="H22" s="1">
-        <v>6272</v>
+      <c r="H22">
+        <v>19392</v>
       </c>
       <c r="I22" s="1">
         <f t="shared" si="4"/>
-        <v>3763.2</v>
+        <v>11635.199999999999</v>
       </c>
       <c r="J22" s="1">
         <f t="shared" si="5"/>
-        <v>10035.200000000001</v>
+        <v>31027.200000000001</v>
       </c>
       <c r="K22" s="1">
         <v>105000</v>
@@ -2568,16 +2574,16 @@
         <f t="shared" si="3"/>
         <v>83800</v>
       </c>
-      <c r="H23" s="1">
-        <v>3920</v>
+      <c r="H23">
+        <v>22992</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" si="4"/>
-        <v>2352</v>
+        <v>13795.199999999999</v>
       </c>
       <c r="J23" s="1">
         <f t="shared" si="5"/>
-        <v>6272</v>
+        <v>36787.200000000004</v>
       </c>
       <c r="K23" s="1">
         <v>105000</v>
@@ -2661,16 +2667,16 @@
         <f t="shared" si="3"/>
         <v>94040</v>
       </c>
-      <c r="H24" s="1">
-        <v>4096</v>
+      <c r="H24">
+        <v>28639.999999999902</v>
       </c>
       <c r="I24" s="1">
         <f t="shared" si="4"/>
-        <v>2457.6</v>
+        <v>17183.999999999942</v>
       </c>
       <c r="J24" s="1">
         <f t="shared" si="5"/>
-        <v>6553.6</v>
+        <v>45823.999999999847</v>
       </c>
       <c r="K24" s="1">
         <v>105000</v>
@@ -2754,16 +2760,16 @@
         <f t="shared" si="3"/>
         <v>80120</v>
       </c>
-      <c r="H25" s="1">
-        <v>5568</v>
+      <c r="H25">
+        <v>20832</v>
       </c>
       <c r="I25" s="1">
         <f t="shared" si="4"/>
-        <v>3340.7999999999997</v>
+        <v>12499.199999999999</v>
       </c>
       <c r="J25" s="1">
         <f t="shared" si="5"/>
-        <v>8908.8000000000011</v>
+        <v>33331.200000000004</v>
       </c>
       <c r="K25" s="1">
         <v>105000</v>
@@ -2847,16 +2853,16 @@
         <f t="shared" si="3"/>
         <v>102760</v>
       </c>
-      <c r="H26" s="1">
-        <v>4352</v>
+      <c r="H26">
+        <v>20784</v>
       </c>
       <c r="I26" s="1">
         <f t="shared" si="4"/>
-        <v>2611.1999999999998</v>
+        <v>12470.4</v>
       </c>
       <c r="J26" s="1">
         <f t="shared" si="5"/>
-        <v>6963.2000000000007</v>
+        <v>33254.400000000001</v>
       </c>
       <c r="K26" s="1">
         <v>105000</v>
@@ -2940,16 +2946,16 @@
         <f t="shared" si="3"/>
         <v>77720</v>
       </c>
-      <c r="H27" s="1">
-        <v>3488</v>
+      <c r="H27">
+        <v>8880</v>
       </c>
       <c r="I27" s="1">
         <f t="shared" si="4"/>
-        <v>2092.7999999999997</v>
+        <v>5328</v>
       </c>
       <c r="J27" s="1">
         <f t="shared" si="5"/>
-        <v>5580.8</v>
+        <v>14208</v>
       </c>
       <c r="K27" s="1">
         <v>105000</v>
@@ -3016,8 +3022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C60A7D1A-E38C-AE45-879F-4A8BE9FD429F}">
   <dimension ref="A1:Y27"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5322,7 +5328,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:I1"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5419,7 +5425,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="5">
-        <v>6.74</v>
+        <v>0</v>
       </c>
       <c r="C4" s="5">
         <v>8.4</v>
@@ -5510,7 +5516,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{151EE3D0-4D23-BB4E-872E-C6226A6170A4}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -5677,4 +5685,444 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDB4CA3D-1AF1-B14C-B9F2-1BFC8231E4F1}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1988</v>
+      </c>
+      <c r="B2">
+        <v>1000000</v>
+      </c>
+      <c r="C2">
+        <v>800000</v>
+      </c>
+      <c r="D2">
+        <v>1500000</v>
+      </c>
+      <c r="E2">
+        <v>16608</v>
+      </c>
+      <c r="F2">
+        <v>6643.2000000000007</v>
+      </c>
+      <c r="G2">
+        <v>41520</v>
+      </c>
+      <c r="H2">
+        <v>16864</v>
+      </c>
+      <c r="I2">
+        <v>10118.4</v>
+      </c>
+      <c r="J2">
+        <v>26982.400000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1989</v>
+      </c>
+      <c r="B3">
+        <v>1000000</v>
+      </c>
+      <c r="C3">
+        <v>800000</v>
+      </c>
+      <c r="D3">
+        <v>1500000</v>
+      </c>
+      <c r="E3">
+        <v>27872</v>
+      </c>
+      <c r="F3">
+        <v>11148.800000000001</v>
+      </c>
+      <c r="G3">
+        <v>69680</v>
+      </c>
+      <c r="H3">
+        <v>13616</v>
+      </c>
+      <c r="I3">
+        <v>8169.5999999999995</v>
+      </c>
+      <c r="J3">
+        <v>21785.600000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1990</v>
+      </c>
+      <c r="B4">
+        <v>1000000</v>
+      </c>
+      <c r="C4">
+        <v>800000</v>
+      </c>
+      <c r="D4">
+        <v>1500000</v>
+      </c>
+      <c r="E4">
+        <v>23504</v>
+      </c>
+      <c r="F4">
+        <v>9401.6</v>
+      </c>
+      <c r="G4">
+        <v>58760</v>
+      </c>
+      <c r="H4">
+        <v>7695.99999999999</v>
+      </c>
+      <c r="I4">
+        <v>4617.599999999994</v>
+      </c>
+      <c r="J4">
+        <v>12313.599999999984</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C002D49C-7408-3941-9CCD-9DB3B7BD832B}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1988</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>48.689</v>
+      </c>
+      <c r="I2">
+        <v>48.689</v>
+      </c>
+      <c r="J2">
+        <v>48.689</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>1989</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>62.747999999999998</v>
+      </c>
+      <c r="I3">
+        <v>62.747999999999998</v>
+      </c>
+      <c r="J3">
+        <v>62.747999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>1990</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>81.164000000000001</v>
+      </c>
+      <c r="I4">
+        <v>81.164000000000001</v>
+      </c>
+      <c r="J4">
+        <v>81.164000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{522E212D-32FB-B643-A8EB-888F61E4EC49}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.65</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>8.4</v>
+      </c>
+      <c r="D4" s="5">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="5">
+        <v>12.9</v>
+      </c>
+      <c r="C5" s="5">
+        <v>7.6</v>
+      </c>
+      <c r="D5" s="5">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="5">
+        <v>128</v>
+      </c>
+      <c r="D6" s="5">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{132A7D3C-FCC3-7447-9323-8649C6633A9B}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Attempt to build a version which includes imports. PP is handled as an import flux to the system every year. The word doc explains the rational for the calculation.
</commit_message>
<xml_diff>
--- a/CaN.Input.Data.xlsx
+++ b/CaN.Input.Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjamin/Documents/Work/CaN/CaN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C5250B6E-4FCB-904B-97A0-72E421B6E439}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{96C27B8E-1F59-704A-8DD1-B8710534E13C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6700" yWindow="2980" windowWidth="28040" windowHeight="17440" activeTab="6" xr2:uid="{273F929D-1BE0-B64B-9C73-B17798356DE2}"/>
+    <workbookView xWindow="6700" yWindow="2980" windowWidth="28040" windowHeight="17440" xr2:uid="{273F929D-1BE0-B64B-9C73-B17798356DE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Biomasses" sheetId="1" r:id="rId1"/>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB5008E-EAEA-734B-A1C9-2CD9D713586D}">
   <dimension ref="A1:Y27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5691,9 +5691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDB4CA3D-1AF1-B14C-B9F2-1BFC8231E4F1}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -5977,7 +5975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{522E212D-32FB-B643-A8EB-888F61E4EC49}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>